<commit_message>
added consult hours insert method
</commit_message>
<xml_diff>
--- a/data/doctorsData.xlsx
+++ b/data/doctorsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\apollo-hospitals\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0881B684-A3A2-4F33-AA74-776D1BFF4F74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076B902B-E382-403A-8CEA-DA77E147511F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2599,9 +2599,6 @@
     <t>09:00 AM - 05:00 PM</t>
   </si>
   <si>
-    <t>08:00 PM - 08:00 AM</t>
-  </si>
-  <si>
     <t>06:00 PM - 07:00 PM</t>
   </si>
   <si>
@@ -2652,6 +2649,9 @@
   </si>
   <si>
     <t>11:00 AM - 12:00 PM</t>
+  </si>
+  <si>
+    <t>08:00 AM - 08:00 PM</t>
   </si>
 </sst>
 </file>
@@ -3174,7 +3174,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB980"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="U94" workbookViewId="0">
+      <selection activeCell="W104" sqref="W104"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3348,7 +3350,7 @@
         <v>33</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>607</v>
@@ -3426,7 +3428,7 @@
         <v>38</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>607</v>
@@ -3506,7 +3508,7 @@
       </c>
       <c r="V4" s="3"/>
       <c r="W4" s="9" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>607</v>
@@ -3588,7 +3590,7 @@
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X5" s="1" t="s">
         <v>607</v>
@@ -3668,7 +3670,7 @@
       </c>
       <c r="V6" s="3"/>
       <c r="W6" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X6" s="1" t="s">
         <v>607</v>
@@ -3750,7 +3752,7 @@
         <v>54</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>607</v>
@@ -3830,7 +3832,7 @@
       </c>
       <c r="V8" s="3"/>
       <c r="W8" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="X8" s="1" t="s">
         <v>607</v>
@@ -3910,7 +3912,7 @@
       </c>
       <c r="V9" s="3"/>
       <c r="W9" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="X9" s="1" t="s">
         <v>607</v>
@@ -3992,7 +3994,7 @@
         <v>67</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="X10" s="1" t="s">
         <v>607</v>
@@ -4072,7 +4074,7 @@
       </c>
       <c r="V11" s="3"/>
       <c r="W11" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="X11" s="1" t="s">
         <v>607</v>
@@ -4150,7 +4152,7 @@
       </c>
       <c r="V12" s="3"/>
       <c r="W12" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X12" s="1" t="s">
         <v>607</v>
@@ -4230,7 +4232,7 @@
       </c>
       <c r="V13" s="3"/>
       <c r="W13" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>607</v>
@@ -4310,7 +4312,7 @@
         <v>84</v>
       </c>
       <c r="W14" s="10" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X14" s="1" t="s">
         <v>607</v>
@@ -4394,7 +4396,7 @@
         <v>89</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="X15" s="1" t="s">
         <v>607</v>
@@ -4476,7 +4478,7 @@
       </c>
       <c r="V16" s="1"/>
       <c r="W16" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X16" s="1" t="s">
         <v>607</v>
@@ -4556,7 +4558,7 @@
         <v>97</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X17" s="1" t="s">
         <v>607</v>
@@ -4640,7 +4642,7 @@
         <v>54</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="X18" s="1" t="s">
         <v>607</v>
@@ -4720,7 +4722,7 @@
       </c>
       <c r="V19" s="1"/>
       <c r="W19" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="X19" s="1" t="s">
         <v>607</v>
@@ -4804,7 +4806,7 @@
         <v>112</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="X20" s="1" t="s">
         <v>607</v>
@@ -4886,7 +4888,7 @@
       </c>
       <c r="V21" s="3"/>
       <c r="W21" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="X21" s="1" t="s">
         <v>607</v>
@@ -4968,7 +4970,7 @@
       </c>
       <c r="V22" s="1"/>
       <c r="W22" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X22" s="1" t="s">
         <v>607</v>
@@ -5046,7 +5048,7 @@
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="X23" s="1" t="s">
         <v>607</v>
@@ -5126,7 +5128,7 @@
       </c>
       <c r="V24" s="3"/>
       <c r="W24" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="X24" s="1" t="s">
         <v>607</v>
@@ -5208,7 +5210,7 @@
         <v>134</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="X25" s="1" t="s">
         <v>607</v>
@@ -5292,7 +5294,7 @@
         <v>139</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="X26" s="1" t="s">
         <v>607</v>
@@ -5374,7 +5376,7 @@
         <v>143</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X27" s="1" t="s">
         <v>607</v>
@@ -5452,7 +5454,7 @@
       </c>
       <c r="V28" s="3"/>
       <c r="W28" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="X28" s="1" t="s">
         <v>607</v>
@@ -5532,7 +5534,7 @@
       </c>
       <c r="V29" s="3"/>
       <c r="W29" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="X29" s="1" t="s">
         <v>608</v>
@@ -5614,7 +5616,7 @@
         <v>156</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="X30" s="1" t="s">
         <v>607</v>
@@ -5694,7 +5696,7 @@
       </c>
       <c r="V31" s="3"/>
       <c r="W31" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X31" s="1" t="s">
         <v>607</v>
@@ -5774,7 +5776,7 @@
       </c>
       <c r="V32" s="1"/>
       <c r="W32" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="X32" s="1" t="s">
         <v>607</v>
@@ -5854,7 +5856,7 @@
       </c>
       <c r="V33" s="3"/>
       <c r="W33" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="X33" s="1" t="s">
         <v>607</v>
@@ -5934,7 +5936,7 @@
       </c>
       <c r="V34" s="3"/>
       <c r="W34" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="X34" s="1" t="s">
         <v>607</v>
@@ -6012,7 +6014,7 @@
       </c>
       <c r="V35" s="3"/>
       <c r="W35" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="X35" s="1" t="s">
         <v>607</v>
@@ -6092,7 +6094,7 @@
       </c>
       <c r="V36" s="3"/>
       <c r="W36" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X36" s="1" t="s">
         <v>607</v>
@@ -6170,7 +6172,7 @@
       </c>
       <c r="V37" s="1"/>
       <c r="W37" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="X37" s="1" t="s">
         <v>607</v>
@@ -6244,7 +6246,7 @@
         <v>496</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X38" s="1" t="s">
         <v>607</v>
@@ -6318,7 +6320,7 @@
       </c>
       <c r="V39" s="4"/>
       <c r="W39" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X39" s="1" t="s">
         <v>607</v>
@@ -6394,7 +6396,7 @@
         <v>485</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X40" s="1" t="s">
         <v>607</v>
@@ -6470,7 +6472,7 @@
       </c>
       <c r="V41" s="4"/>
       <c r="W41" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="X41" s="1" t="s">
         <v>607</v>
@@ -6544,7 +6546,7 @@
       </c>
       <c r="V42" s="1"/>
       <c r="W42" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X42" s="1" t="s">
         <v>607</v>
@@ -6618,7 +6620,7 @@
       </c>
       <c r="V43" s="1"/>
       <c r="W43" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="X43" s="1" t="s">
         <v>607</v>
@@ -6692,7 +6694,7 @@
       </c>
       <c r="V44" s="2"/>
       <c r="W44" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X44" s="1" t="s">
         <v>607</v>
@@ -6768,7 +6770,7 @@
       </c>
       <c r="V45" s="2"/>
       <c r="W45" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X45" s="1" t="s">
         <v>607</v>
@@ -6842,7 +6844,7 @@
       </c>
       <c r="V46" s="2"/>
       <c r="W46" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X46" s="1" t="s">
         <v>607</v>
@@ -6918,7 +6920,7 @@
       </c>
       <c r="V47" s="2"/>
       <c r="W47" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X47" s="1" t="s">
         <v>607</v>
@@ -6992,7 +6994,7 @@
       </c>
       <c r="V48" s="2"/>
       <c r="W48" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X48" s="1" t="s">
         <v>607</v>
@@ -7066,7 +7068,7 @@
       </c>
       <c r="V49" s="2"/>
       <c r="W49" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X49" s="1" t="s">
         <v>607</v>
@@ -7140,7 +7142,7 @@
       </c>
       <c r="V50" s="2"/>
       <c r="W50" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="X50" s="1" t="s">
         <v>607</v>
@@ -7214,7 +7216,7 @@
       </c>
       <c r="V51" s="2"/>
       <c r="W51" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X51" s="1" t="s">
         <v>607</v>
@@ -7290,7 +7292,7 @@
       </c>
       <c r="V52" s="2"/>
       <c r="W52" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X52" s="1" t="s">
         <v>607</v>
@@ -7364,7 +7366,7 @@
       </c>
       <c r="V53" s="2"/>
       <c r="W53" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X53" s="1" t="s">
         <v>607</v>
@@ -7440,7 +7442,7 @@
         <v>422</v>
       </c>
       <c r="W54" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X54" s="1" t="s">
         <v>607</v>
@@ -7518,7 +7520,7 @@
         <v>416</v>
       </c>
       <c r="W55" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X55" s="1" t="s">
         <v>607</v>
@@ -7594,7 +7596,7 @@
         <v>411</v>
       </c>
       <c r="W56" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="X56" s="1" t="s">
         <v>607</v>
@@ -7666,7 +7668,7 @@
       </c>
       <c r="V57" s="2"/>
       <c r="W57" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="X57" s="1" t="s">
         <v>607</v>
@@ -7744,7 +7746,7 @@
         <v>400</v>
       </c>
       <c r="W58" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X58" s="1" t="s">
         <v>607</v>
@@ -7822,7 +7824,7 @@
         <v>394</v>
       </c>
       <c r="W59" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X59" s="1" t="s">
         <v>607</v>
@@ -7898,7 +7900,7 @@
         <v>388</v>
       </c>
       <c r="W60" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="X60" s="1" t="s">
         <v>607</v>
@@ -7974,7 +7976,7 @@
         <v>381</v>
       </c>
       <c r="W61" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X61" s="1" t="s">
         <v>607</v>
@@ -8050,7 +8052,7 @@
       </c>
       <c r="V62" s="2"/>
       <c r="W62" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X62" s="1" t="s">
         <v>607</v>
@@ -8128,7 +8130,7 @@
         <v>369</v>
       </c>
       <c r="W63" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X63" s="1" t="s">
         <v>607</v>
@@ -8204,7 +8206,7 @@
         <v>364</v>
       </c>
       <c r="W64" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X64" s="1" t="s">
         <v>607</v>
@@ -8278,7 +8280,7 @@
         <v>359</v>
       </c>
       <c r="W65" s="5" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="X65" s="1" t="s">
         <v>607</v>
@@ -8354,7 +8356,7 @@
         <v>352</v>
       </c>
       <c r="W66" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X66" s="1" t="s">
         <v>607</v>
@@ -8430,7 +8432,7 @@
         <v>345</v>
       </c>
       <c r="W67" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X67" s="1" t="s">
         <v>607</v>
@@ -8504,7 +8506,7 @@
       </c>
       <c r="V68" s="2"/>
       <c r="W68" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X68" s="1" t="s">
         <v>607</v>
@@ -8580,7 +8582,7 @@
         <v>334</v>
       </c>
       <c r="W69" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="X69" s="1" t="s">
         <v>607</v>
@@ -8656,7 +8658,7 @@
         <v>329</v>
       </c>
       <c r="W70" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X70" s="1" t="s">
         <v>607</v>
@@ -8732,7 +8734,7 @@
         <v>323</v>
       </c>
       <c r="W71" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X71" s="1" t="s">
         <v>607</v>
@@ -8808,7 +8810,7 @@
         <v>317</v>
       </c>
       <c r="W72" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X72" s="1" t="s">
         <v>607</v>
@@ -8882,7 +8884,7 @@
       </c>
       <c r="V73" s="2"/>
       <c r="W73" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X73" s="1" t="s">
         <v>607</v>
@@ -8956,7 +8958,7 @@
       </c>
       <c r="V74" s="2"/>
       <c r="W74" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X74" s="1" t="s">
         <v>607</v>
@@ -9032,7 +9034,7 @@
         <v>301</v>
       </c>
       <c r="W75" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X75" s="1" t="s">
         <v>607</v>
@@ -9110,7 +9112,7 @@
         <v>294</v>
       </c>
       <c r="W76" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X76" s="1" t="s">
         <v>607</v>
@@ -9188,7 +9190,7 @@
         <v>287</v>
       </c>
       <c r="W77" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X77" s="1" t="s">
         <v>607</v>
@@ -9264,7 +9266,7 @@
         <v>281</v>
       </c>
       <c r="W78" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="X78" s="1" t="s">
         <v>607</v>
@@ -9340,7 +9342,7 @@
         <v>274</v>
       </c>
       <c r="W79" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="X79" s="1" t="s">
         <v>607</v>
@@ -9418,7 +9420,7 @@
         <v>266</v>
       </c>
       <c r="W80" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X80" s="1" t="s">
         <v>607</v>
@@ -9494,7 +9496,7 @@
         <v>259</v>
       </c>
       <c r="W81" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="X81" s="1" t="s">
         <v>607</v>
@@ -9570,7 +9572,7 @@
         <v>253</v>
       </c>
       <c r="W82" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X82" s="1" t="s">
         <v>607</v>
@@ -9648,7 +9650,7 @@
         <v>247</v>
       </c>
       <c r="W83" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="X83" s="1" t="s">
         <v>607</v>
@@ -9724,7 +9726,7 @@
         <v>240</v>
       </c>
       <c r="W84" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="X84" s="1" t="s">
         <v>607</v>
@@ -9800,7 +9802,7 @@
         <v>233</v>
       </c>
       <c r="W85" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X85" s="1" t="s">
         <v>607</v>
@@ -9876,7 +9878,7 @@
         <v>226</v>
       </c>
       <c r="W86" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X86" s="1" t="s">
         <v>607</v>
@@ -9952,7 +9954,7 @@
         <v>218</v>
       </c>
       <c r="W87" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="X87" s="1" t="s">
         <v>606</v>
@@ -11024,7 +11026,7 @@
       <c r="U103" s="14"/>
       <c r="V103" s="13"/>
       <c r="W103" s="14" t="s">
-        <v>838</v>
+        <v>855</v>
       </c>
       <c r="X103" s="1" t="s">
         <v>606</v>

</xml_diff>